<commit_message>
Revert "Fix dates bug and country codes bug"
This reverts commit 84d45b68d0bf080c09ddf84d40ae315cf44129fa.
</commit_message>
<xml_diff>
--- a/Data/Data_Raw/Country codes & metadata/wbcodes_equiv_UN.xlsx
+++ b/Data/Data_Raw/Country codes & metadata/wbcodes_equiv_UN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laboral\World Bank\Data-Portal-Brief-Generator\Data\Data_Raw\Country codes &amp; metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\llohi\Documents\WB\Data Portal\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE543396-44FA-4A97-A65B-0587BD2950E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8937A45F-B73F-4B9A-BDD0-C2A60FDE7970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{35768C06-BC63-4492-A96D-3D68320C9AFB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{35768C06-BC63-4492-A96D-3D68320C9AFB}"/>
   </bookViews>
   <sheets>
     <sheet name="UN" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="439">
   <si>
     <t>wbname</t>
   </si>
@@ -374,6 +374,9 @@
     <t>Congo, Dem. Rep.</t>
   </si>
   <si>
+    <t>ZAR</t>
+  </si>
+  <si>
     <t>DNK</t>
   </si>
   <si>
@@ -975,6 +978,9 @@
   </si>
   <si>
     <t>Romania</t>
+  </si>
+  <si>
+    <t>ROM</t>
   </si>
   <si>
     <t>RUS</t>
@@ -1402,7 +1408,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1700,18 +1706,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9DC979A-84E7-47B6-A734-973D4F9D0964}">
   <dimension ref="A1:D203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
-      <selection activeCell="D147" sqref="D147"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="B1" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1720,7 +1726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1734,7 +1740,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1748,7 +1754,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1762,7 +1768,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1776,7 +1782,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1790,7 +1796,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1804,7 +1810,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1818,7 +1824,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1832,7 +1838,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1846,7 +1852,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1860,7 +1866,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1874,7 +1880,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1888,7 +1894,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -1902,7 +1908,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -1916,7 +1922,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1930,7 +1936,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -1944,7 +1950,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -1958,7 +1964,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -1972,7 +1978,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -1986,7 +1992,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -2000,7 +2006,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -2014,7 +2020,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -2028,7 +2034,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>49</v>
       </c>
@@ -2042,7 +2048,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>51</v>
       </c>
@@ -2056,7 +2062,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>53</v>
       </c>
@@ -2070,7 +2076,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>55</v>
       </c>
@@ -2084,7 +2090,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>57</v>
       </c>
@@ -2098,7 +2104,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>60</v>
       </c>
@@ -2112,7 +2118,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>62</v>
       </c>
@@ -2126,7 +2132,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>64</v>
       </c>
@@ -2140,7 +2146,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>66</v>
       </c>
@@ -2154,7 +2160,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>69</v>
       </c>
@@ -2168,7 +2174,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>71</v>
       </c>
@@ -2182,7 +2188,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>73</v>
       </c>
@@ -2196,7 +2202,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>75</v>
       </c>
@@ -2210,7 +2216,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>77</v>
       </c>
@@ -2224,7 +2230,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>79</v>
       </c>
@@ -2238,7 +2244,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>81</v>
       </c>
@@ -2252,7 +2258,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>83</v>
       </c>
@@ -2266,7 +2272,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>85</v>
       </c>
@@ -2280,7 +2286,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>87</v>
       </c>
@@ -2294,7 +2300,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>90</v>
       </c>
@@ -2308,7 +2314,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>92</v>
       </c>
@@ -2322,7 +2328,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>94</v>
       </c>
@@ -2336,7 +2342,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>97</v>
       </c>
@@ -2350,7 +2356,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>99</v>
       </c>
@@ -2364,7 +2370,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>101</v>
       </c>
@@ -2378,7 +2384,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>103</v>
       </c>
@@ -2392,7 +2398,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>106</v>
       </c>
@@ -2406,7 +2412,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>109</v>
       </c>
@@ -2417,2135 +2423,2135 @@
         <v>111</v>
       </c>
       <c r="D51" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B52" t="s">
+        <v>114</v>
+      </c>
+      <c r="C52" t="s">
+        <v>114</v>
+      </c>
+      <c r="D52" t="s">
         <v>113</v>
       </c>
-      <c r="C52" t="s">
-        <v>113</v>
-      </c>
-      <c r="D52" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B53" t="s">
+        <v>116</v>
+      </c>
+      <c r="C53" t="s">
+        <v>116</v>
+      </c>
+      <c r="D53" t="s">
         <v>115</v>
       </c>
-      <c r="C53" t="s">
-        <v>115</v>
-      </c>
-      <c r="D53" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B54" t="s">
+        <v>118</v>
+      </c>
+      <c r="C54" t="s">
+        <v>118</v>
+      </c>
+      <c r="D54" t="s">
         <v>117</v>
       </c>
-      <c r="C54" t="s">
-        <v>117</v>
-      </c>
-      <c r="D54" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B55" t="s">
+        <v>120</v>
+      </c>
+      <c r="C55" t="s">
+        <v>120</v>
+      </c>
+      <c r="D55" t="s">
         <v>119</v>
       </c>
-      <c r="C55" t="s">
-        <v>119</v>
-      </c>
-      <c r="D55" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B56" t="s">
+        <v>122</v>
+      </c>
+      <c r="C56" t="s">
+        <v>122</v>
+      </c>
+      <c r="D56" t="s">
         <v>121</v>
       </c>
-      <c r="C56" t="s">
-        <v>121</v>
-      </c>
-      <c r="D56" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B57" t="s">
+        <v>124</v>
+      </c>
+      <c r="C57" t="s">
+        <v>125</v>
+      </c>
+      <c r="D57" t="s">
         <v>123</v>
       </c>
-      <c r="C57" t="s">
-        <v>124</v>
-      </c>
-      <c r="D57" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B58" t="s">
+        <v>127</v>
+      </c>
+      <c r="C58" t="s">
+        <v>127</v>
+      </c>
+      <c r="D58" t="s">
         <v>126</v>
       </c>
-      <c r="C58" t="s">
-        <v>126</v>
-      </c>
-      <c r="D58" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B59" t="s">
+        <v>129</v>
+      </c>
+      <c r="C59" t="s">
+        <v>129</v>
+      </c>
+      <c r="D59" t="s">
         <v>128</v>
       </c>
-      <c r="C59" t="s">
-        <v>128</v>
-      </c>
-      <c r="D59" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B60" t="s">
+        <v>131</v>
+      </c>
+      <c r="C60" t="s">
+        <v>131</v>
+      </c>
+      <c r="D60" t="s">
         <v>130</v>
       </c>
-      <c r="C60" t="s">
-        <v>130</v>
-      </c>
-      <c r="D60" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B61" t="s">
+        <v>133</v>
+      </c>
+      <c r="C61" t="s">
+        <v>133</v>
+      </c>
+      <c r="D61" t="s">
         <v>132</v>
       </c>
-      <c r="C61" t="s">
-        <v>132</v>
-      </c>
-      <c r="D61" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B62" t="s">
+        <v>135</v>
+      </c>
+      <c r="C62" t="s">
+        <v>136</v>
+      </c>
+      <c r="D62" t="s">
         <v>134</v>
       </c>
-      <c r="C62" t="s">
-        <v>135</v>
-      </c>
-      <c r="D62" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B63" t="s">
+        <v>138</v>
+      </c>
+      <c r="C63" t="s">
+        <v>138</v>
+      </c>
+      <c r="D63" t="s">
         <v>137</v>
       </c>
-      <c r="C63" t="s">
-        <v>137</v>
-      </c>
-      <c r="D63" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B64" t="s">
+        <v>140</v>
+      </c>
+      <c r="C64" t="s">
+        <v>140</v>
+      </c>
+      <c r="D64" t="s">
         <v>139</v>
       </c>
-      <c r="C64" t="s">
-        <v>139</v>
-      </c>
-      <c r="D64" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B65" t="s">
+        <v>142</v>
+      </c>
+      <c r="C65" t="s">
+        <v>142</v>
+      </c>
+      <c r="D65" t="s">
         <v>141</v>
       </c>
-      <c r="C65" t="s">
-        <v>141</v>
-      </c>
-      <c r="D65" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B66" t="s">
+        <v>144</v>
+      </c>
+      <c r="C66" t="s">
+        <v>144</v>
+      </c>
+      <c r="D66" t="s">
         <v>143</v>
       </c>
-      <c r="C66" t="s">
-        <v>143</v>
-      </c>
-      <c r="D66" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B67" t="s">
+        <v>146</v>
+      </c>
+      <c r="C67" t="s">
+        <v>147</v>
+      </c>
+      <c r="D67" t="s">
         <v>145</v>
       </c>
-      <c r="C67" t="s">
-        <v>146</v>
-      </c>
-      <c r="D67" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B68" t="s">
+        <v>149</v>
+      </c>
+      <c r="C68" t="s">
+        <v>149</v>
+      </c>
+      <c r="D68" t="s">
         <v>148</v>
       </c>
-      <c r="C68" t="s">
-        <v>148</v>
-      </c>
-      <c r="D68" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B69" t="s">
+        <v>151</v>
+      </c>
+      <c r="C69" t="s">
+        <v>151</v>
+      </c>
+      <c r="D69" t="s">
         <v>150</v>
       </c>
-      <c r="C69" t="s">
-        <v>150</v>
-      </c>
-      <c r="D69" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B70" t="s">
+        <v>153</v>
+      </c>
+      <c r="C70" t="s">
+        <v>153</v>
+      </c>
+      <c r="D70" t="s">
         <v>152</v>
       </c>
-      <c r="C70" t="s">
-        <v>152</v>
-      </c>
-      <c r="D70" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B71" t="s">
+        <v>155</v>
+      </c>
+      <c r="C71" t="s">
+        <v>155</v>
+      </c>
+      <c r="D71" t="s">
         <v>154</v>
       </c>
-      <c r="C71" t="s">
-        <v>154</v>
-      </c>
-      <c r="D71" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B72" t="s">
+        <v>157</v>
+      </c>
+      <c r="C72" t="s">
+        <v>157</v>
+      </c>
+      <c r="D72" t="s">
         <v>156</v>
       </c>
-      <c r="C72" t="s">
-        <v>156</v>
-      </c>
-      <c r="D72" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B73" t="s">
+        <v>159</v>
+      </c>
+      <c r="C73" t="s">
+        <v>159</v>
+      </c>
+      <c r="D73" t="s">
         <v>158</v>
       </c>
-      <c r="C73" t="s">
-        <v>158</v>
-      </c>
-      <c r="D73" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B74" t="s">
+        <v>161</v>
+      </c>
+      <c r="C74" t="s">
+        <v>161</v>
+      </c>
+      <c r="D74" t="s">
         <v>160</v>
       </c>
-      <c r="C74" t="s">
-        <v>160</v>
-      </c>
-      <c r="D74" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B75" t="s">
+        <v>163</v>
+      </c>
+      <c r="C75" t="s">
+        <v>163</v>
+      </c>
+      <c r="D75" t="s">
         <v>162</v>
       </c>
-      <c r="C75" t="s">
-        <v>162</v>
-      </c>
-      <c r="D75" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B76" t="s">
+        <v>165</v>
+      </c>
+      <c r="C76" t="s">
+        <v>165</v>
+      </c>
+      <c r="D76" t="s">
         <v>164</v>
       </c>
-      <c r="C76" t="s">
-        <v>164</v>
-      </c>
-      <c r="D76" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B77" t="s">
+        <v>167</v>
+      </c>
+      <c r="C77" t="s">
+        <v>167</v>
+      </c>
+      <c r="D77" t="s">
         <v>166</v>
       </c>
-      <c r="C77" t="s">
-        <v>166</v>
-      </c>
-      <c r="D77" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B78" t="s">
+        <v>169</v>
+      </c>
+      <c r="C78" t="s">
+        <v>169</v>
+      </c>
+      <c r="D78" t="s">
         <v>168</v>
       </c>
-      <c r="C78" t="s">
-        <v>168</v>
-      </c>
-      <c r="D78" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B79" t="s">
+        <v>171</v>
+      </c>
+      <c r="C79" t="s">
+        <v>171</v>
+      </c>
+      <c r="D79" t="s">
         <v>170</v>
       </c>
-      <c r="C79" t="s">
-        <v>170</v>
-      </c>
-      <c r="D79" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B80" t="s">
+        <v>173</v>
+      </c>
+      <c r="C80" t="s">
+        <v>173</v>
+      </c>
+      <c r="D80" t="s">
         <v>172</v>
       </c>
-      <c r="C80" t="s">
-        <v>172</v>
-      </c>
-      <c r="D80" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B81" t="s">
+        <v>175</v>
+      </c>
+      <c r="C81" t="s">
+        <v>175</v>
+      </c>
+      <c r="D81" t="s">
         <v>174</v>
       </c>
-      <c r="C81" t="s">
-        <v>174</v>
-      </c>
-      <c r="D81" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B82" t="s">
+        <v>177</v>
+      </c>
+      <c r="C82" t="s">
+        <v>177</v>
+      </c>
+      <c r="D82" t="s">
         <v>176</v>
       </c>
-      <c r="C82" t="s">
-        <v>176</v>
-      </c>
-      <c r="D82" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B83" t="s">
+        <v>179</v>
+      </c>
+      <c r="C83" t="s">
+        <v>179</v>
+      </c>
+      <c r="D83" t="s">
         <v>178</v>
       </c>
-      <c r="C83" t="s">
-        <v>178</v>
-      </c>
-      <c r="D83" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B84" t="s">
+        <v>181</v>
+      </c>
+      <c r="C84" t="s">
+        <v>182</v>
+      </c>
+      <c r="D84" t="s">
         <v>180</v>
       </c>
-      <c r="C84" t="s">
-        <v>181</v>
-      </c>
-      <c r="D84" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B85" t="s">
+        <v>184</v>
+      </c>
+      <c r="C85" t="s">
+        <v>184</v>
+      </c>
+      <c r="D85" t="s">
         <v>183</v>
       </c>
-      <c r="C85" t="s">
-        <v>183</v>
-      </c>
-      <c r="D85" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B86" t="s">
+        <v>186</v>
+      </c>
+      <c r="C86" t="s">
+        <v>186</v>
+      </c>
+      <c r="D86" t="s">
         <v>185</v>
       </c>
-      <c r="C86" t="s">
-        <v>185</v>
-      </c>
-      <c r="D86" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B87" t="s">
+        <v>188</v>
+      </c>
+      <c r="C87" t="s">
+        <v>188</v>
+      </c>
+      <c r="D87" t="s">
         <v>187</v>
       </c>
-      <c r="C87" t="s">
-        <v>187</v>
-      </c>
-      <c r="D87" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B88" t="s">
+        <v>190</v>
+      </c>
+      <c r="C88" t="s">
+        <v>190</v>
+      </c>
+      <c r="D88" t="s">
         <v>189</v>
       </c>
-      <c r="C88" t="s">
-        <v>189</v>
-      </c>
-      <c r="D88" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B89" t="s">
+        <v>192</v>
+      </c>
+      <c r="C89" t="s">
+        <v>192</v>
+      </c>
+      <c r="D89" t="s">
         <v>191</v>
       </c>
-      <c r="C89" t="s">
-        <v>191</v>
-      </c>
-      <c r="D89" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B90" t="s">
+        <v>194</v>
+      </c>
+      <c r="C90" t="s">
+        <v>194</v>
+      </c>
+      <c r="D90" t="s">
         <v>193</v>
       </c>
-      <c r="C90" t="s">
-        <v>193</v>
-      </c>
-      <c r="D90" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B91" t="s">
+        <v>196</v>
+      </c>
+      <c r="C91" t="s">
+        <v>196</v>
+      </c>
+      <c r="D91" t="s">
         <v>195</v>
       </c>
-      <c r="C91" t="s">
-        <v>195</v>
-      </c>
-      <c r="D91" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B92" t="s">
+        <v>198</v>
+      </c>
+      <c r="C92" t="s">
+        <v>198</v>
+      </c>
+      <c r="D92" t="s">
         <v>197</v>
       </c>
-      <c r="C92" t="s">
-        <v>197</v>
-      </c>
-      <c r="D92" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B93" t="s">
+        <v>200</v>
+      </c>
+      <c r="C93" t="s">
+        <v>200</v>
+      </c>
+      <c r="D93" t="s">
         <v>199</v>
       </c>
-      <c r="C93" t="s">
-        <v>199</v>
-      </c>
-      <c r="D93" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B94" t="s">
+        <v>202</v>
+      </c>
+      <c r="C94" t="s">
+        <v>202</v>
+      </c>
+      <c r="D94" t="s">
         <v>201</v>
       </c>
-      <c r="C94" t="s">
-        <v>201</v>
-      </c>
-      <c r="D94" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B95" t="s">
+        <v>204</v>
+      </c>
+      <c r="C95" t="s">
+        <v>204</v>
+      </c>
+      <c r="D95" t="s">
         <v>203</v>
       </c>
-      <c r="C95" t="s">
-        <v>203</v>
-      </c>
-      <c r="D95" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B96" t="s">
+        <v>206</v>
+      </c>
+      <c r="C96" t="s">
+        <v>207</v>
+      </c>
+      <c r="D96" t="s">
         <v>205</v>
       </c>
-      <c r="C96" t="s">
-        <v>206</v>
-      </c>
-      <c r="D96" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B97" t="s">
+        <v>209</v>
+      </c>
+      <c r="C97" t="s">
+        <v>210</v>
+      </c>
+      <c r="D97" t="s">
         <v>208</v>
       </c>
-      <c r="C97" t="s">
-        <v>209</v>
-      </c>
-      <c r="D97" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B98" t="s">
+        <v>212</v>
+      </c>
+      <c r="C98" t="s">
+        <v>212</v>
+      </c>
+      <c r="D98" t="s">
         <v>211</v>
       </c>
-      <c r="C98" t="s">
-        <v>211</v>
-      </c>
-      <c r="D98" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B99" t="s">
+        <v>214</v>
+      </c>
+      <c r="C99" t="s">
+        <v>214</v>
+      </c>
+      <c r="D99" t="s">
         <v>213</v>
       </c>
-      <c r="C99" t="s">
-        <v>213</v>
-      </c>
-      <c r="D99" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B100" t="s">
+        <v>216</v>
+      </c>
+      <c r="C100" t="s">
+        <v>216</v>
+      </c>
+      <c r="D100" t="s">
         <v>215</v>
       </c>
-      <c r="C100" t="s">
-        <v>215</v>
-      </c>
-      <c r="D100" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B101" t="s">
+        <v>218</v>
+      </c>
+      <c r="C101" t="s">
+        <v>218</v>
+      </c>
+      <c r="D101" t="s">
         <v>217</v>
       </c>
-      <c r="C101" t="s">
-        <v>217</v>
-      </c>
-      <c r="D101" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B102" t="s">
+        <v>220</v>
+      </c>
+      <c r="C102" t="s">
+        <v>220</v>
+      </c>
+      <c r="D102" t="s">
         <v>219</v>
       </c>
-      <c r="C102" t="s">
-        <v>219</v>
-      </c>
-      <c r="D102" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B103" t="s">
+        <v>222</v>
+      </c>
+      <c r="C103" t="s">
+        <v>222</v>
+      </c>
+      <c r="D103" t="s">
         <v>221</v>
       </c>
-      <c r="C103" t="s">
-        <v>221</v>
-      </c>
-      <c r="D103" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B104" t="s">
+        <v>224</v>
+      </c>
+      <c r="C104" t="s">
+        <v>224</v>
+      </c>
+      <c r="D104" t="s">
         <v>223</v>
       </c>
-      <c r="C104" t="s">
-        <v>223</v>
-      </c>
-      <c r="D104" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B105" t="s">
+        <v>226</v>
+      </c>
+      <c r="C105" t="s">
+        <v>226</v>
+      </c>
+      <c r="D105" t="s">
         <v>225</v>
       </c>
-      <c r="C105" t="s">
-        <v>225</v>
-      </c>
-      <c r="D105" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B106" t="s">
+        <v>228</v>
+      </c>
+      <c r="C106" t="s">
+        <v>228</v>
+      </c>
+      <c r="D106" t="s">
         <v>227</v>
       </c>
-      <c r="C106" t="s">
-        <v>227</v>
-      </c>
-      <c r="D106" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B107" t="s">
+        <v>230</v>
+      </c>
+      <c r="C107" t="s">
+        <v>230</v>
+      </c>
+      <c r="D107" t="s">
         <v>229</v>
       </c>
-      <c r="C107" t="s">
-        <v>229</v>
-      </c>
-      <c r="D107" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B108" t="s">
+        <v>232</v>
+      </c>
+      <c r="C108" t="s">
+        <v>232</v>
+      </c>
+      <c r="D108" t="s">
         <v>231</v>
       </c>
-      <c r="C108" t="s">
-        <v>231</v>
-      </c>
-      <c r="D108" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B109" t="s">
+        <v>234</v>
+      </c>
+      <c r="C109" t="s">
+        <v>234</v>
+      </c>
+      <c r="D109" t="s">
         <v>233</v>
       </c>
-      <c r="C109" t="s">
-        <v>233</v>
-      </c>
-      <c r="D109" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B110" t="s">
+        <v>236</v>
+      </c>
+      <c r="C110" t="s">
+        <v>236</v>
+      </c>
+      <c r="D110" t="s">
         <v>235</v>
       </c>
-      <c r="C110" t="s">
-        <v>235</v>
-      </c>
-      <c r="D110" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B111" t="s">
+        <v>238</v>
+      </c>
+      <c r="C111" t="s">
+        <v>238</v>
+      </c>
+      <c r="D111" t="s">
         <v>237</v>
       </c>
-      <c r="C111" t="s">
-        <v>237</v>
-      </c>
-      <c r="D111" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B112" t="s">
+        <v>240</v>
+      </c>
+      <c r="C112" t="s">
+        <v>240</v>
+      </c>
+      <c r="D112" t="s">
         <v>239</v>
       </c>
-      <c r="C112" t="s">
-        <v>239</v>
-      </c>
-      <c r="D112" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B113" t="s">
+        <v>242</v>
+      </c>
+      <c r="C113" t="s">
+        <v>242</v>
+      </c>
+      <c r="D113" t="s">
         <v>241</v>
       </c>
-      <c r="C113" t="s">
-        <v>241</v>
-      </c>
-      <c r="D113" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B114" t="s">
+        <v>244</v>
+      </c>
+      <c r="C114" t="s">
+        <v>244</v>
+      </c>
+      <c r="D114" t="s">
         <v>243</v>
       </c>
-      <c r="C114" t="s">
-        <v>243</v>
-      </c>
-      <c r="D114" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B115" t="s">
+        <v>246</v>
+      </c>
+      <c r="C115" t="s">
+        <v>246</v>
+      </c>
+      <c r="D115" t="s">
         <v>245</v>
       </c>
-      <c r="C115" t="s">
-        <v>245</v>
-      </c>
-      <c r="D115" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B116" t="s">
+        <v>248</v>
+      </c>
+      <c r="C116" t="s">
+        <v>249</v>
+      </c>
+      <c r="D116" t="s">
         <v>247</v>
       </c>
-      <c r="C116" t="s">
-        <v>248</v>
-      </c>
-      <c r="D116" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B117" t="s">
+        <v>251</v>
+      </c>
+      <c r="C117" t="s">
+        <v>251</v>
+      </c>
+      <c r="D117" t="s">
         <v>250</v>
       </c>
-      <c r="C117" t="s">
-        <v>250</v>
-      </c>
-      <c r="D117" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B118" t="s">
+        <v>253</v>
+      </c>
+      <c r="C118" t="s">
+        <v>253</v>
+      </c>
+      <c r="D118" t="s">
         <v>252</v>
       </c>
-      <c r="C118" t="s">
-        <v>252</v>
-      </c>
-      <c r="D118" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B119" t="s">
-        <v>254</v>
-      </c>
-      <c r="C119" t="s">
-        <v>254</v>
-      </c>
-      <c r="D119" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
+        <v>255</v>
+      </c>
+      <c r="C119" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D119" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B120" t="s">
+        <v>257</v>
+      </c>
+      <c r="C120" t="s">
+        <v>257</v>
+      </c>
+      <c r="D120" t="s">
         <v>256</v>
       </c>
-      <c r="C120" t="s">
-        <v>256</v>
-      </c>
-      <c r="D120" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B121" t="s">
+        <v>259</v>
+      </c>
+      <c r="C121" t="s">
+        <v>259</v>
+      </c>
+      <c r="D121" t="s">
         <v>258</v>
       </c>
-      <c r="C121" t="s">
-        <v>258</v>
-      </c>
-      <c r="D121" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B122" t="s">
+        <v>261</v>
+      </c>
+      <c r="C122" t="s">
+        <v>261</v>
+      </c>
+      <c r="D122" t="s">
         <v>260</v>
       </c>
-      <c r="C122" t="s">
-        <v>260</v>
-      </c>
-      <c r="D122" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B123" t="s">
+        <v>263</v>
+      </c>
+      <c r="C123" t="s">
+        <v>263</v>
+      </c>
+      <c r="D123" t="s">
         <v>262</v>
       </c>
-      <c r="C123" t="s">
-        <v>262</v>
-      </c>
-      <c r="D123" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B124" t="s">
+        <v>265</v>
+      </c>
+      <c r="C124" t="s">
+        <v>265</v>
+      </c>
+      <c r="D124" t="s">
         <v>264</v>
       </c>
-      <c r="C124" t="s">
-        <v>264</v>
-      </c>
-      <c r="D124" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B125" t="s">
+        <v>267</v>
+      </c>
+      <c r="C125" t="s">
+        <v>267</v>
+      </c>
+      <c r="D125" t="s">
         <v>266</v>
       </c>
-      <c r="C125" t="s">
-        <v>266</v>
-      </c>
-      <c r="D125" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B126" t="s">
+        <v>269</v>
+      </c>
+      <c r="C126" t="s">
+        <v>269</v>
+      </c>
+      <c r="D126" t="s">
         <v>268</v>
       </c>
-      <c r="C126" t="s">
-        <v>268</v>
-      </c>
-      <c r="D126" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B127" t="s">
+        <v>271</v>
+      </c>
+      <c r="C127" t="s">
+        <v>271</v>
+      </c>
+      <c r="D127" t="s">
         <v>270</v>
       </c>
-      <c r="C127" t="s">
-        <v>270</v>
-      </c>
-      <c r="D127" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B128" t="s">
+        <v>273</v>
+      </c>
+      <c r="C128" t="s">
+        <v>273</v>
+      </c>
+      <c r="D128" t="s">
         <v>272</v>
       </c>
-      <c r="C128" t="s">
-        <v>272</v>
-      </c>
-      <c r="D128" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B129" t="s">
+        <v>275</v>
+      </c>
+      <c r="C129" t="s">
+        <v>275</v>
+      </c>
+      <c r="D129" t="s">
         <v>274</v>
       </c>
-      <c r="C129" t="s">
-        <v>274</v>
-      </c>
-      <c r="D129" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B130" t="s">
+        <v>277</v>
+      </c>
+      <c r="C130" t="s">
+        <v>277</v>
+      </c>
+      <c r="D130" t="s">
         <v>276</v>
       </c>
-      <c r="C130" t="s">
-        <v>276</v>
-      </c>
-      <c r="D130" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B131" t="s">
+        <v>279</v>
+      </c>
+      <c r="C131" t="s">
+        <v>279</v>
+      </c>
+      <c r="D131" t="s">
         <v>278</v>
       </c>
-      <c r="C131" t="s">
-        <v>278</v>
-      </c>
-      <c r="D131" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B132" t="s">
+        <v>281</v>
+      </c>
+      <c r="C132" t="s">
+        <v>281</v>
+      </c>
+      <c r="D132" t="s">
         <v>280</v>
       </c>
-      <c r="C132" t="s">
-        <v>280</v>
-      </c>
-      <c r="D132" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B133" t="s">
+        <v>283</v>
+      </c>
+      <c r="C133" t="s">
+        <v>283</v>
+      </c>
+      <c r="D133" t="s">
         <v>282</v>
       </c>
-      <c r="C133" t="s">
-        <v>282</v>
-      </c>
-      <c r="D133" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B134" t="s">
+        <v>285</v>
+      </c>
+      <c r="C134" t="s">
+        <v>285</v>
+      </c>
+      <c r="D134" t="s">
         <v>284</v>
       </c>
-      <c r="C134" t="s">
-        <v>284</v>
-      </c>
-      <c r="D134" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B135" t="s">
+        <v>287</v>
+      </c>
+      <c r="C135" t="s">
+        <v>287</v>
+      </c>
+      <c r="D135" t="s">
         <v>286</v>
       </c>
-      <c r="C135" t="s">
-        <v>286</v>
-      </c>
-      <c r="D135" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B136" t="s">
+        <v>289</v>
+      </c>
+      <c r="C136" t="s">
+        <v>289</v>
+      </c>
+      <c r="D136" t="s">
         <v>288</v>
       </c>
-      <c r="C136" t="s">
-        <v>288</v>
-      </c>
-      <c r="D136" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B137" t="s">
+        <v>291</v>
+      </c>
+      <c r="C137" t="s">
+        <v>291</v>
+      </c>
+      <c r="D137" t="s">
         <v>290</v>
       </c>
-      <c r="C137" t="s">
-        <v>290</v>
-      </c>
-      <c r="D137" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B138" t="s">
+        <v>293</v>
+      </c>
+      <c r="C138" t="s">
+        <v>293</v>
+      </c>
+      <c r="D138" t="s">
         <v>292</v>
       </c>
-      <c r="C138" t="s">
-        <v>292</v>
-      </c>
-      <c r="D138" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B139" t="s">
+        <v>295</v>
+      </c>
+      <c r="C139" t="s">
+        <v>295</v>
+      </c>
+      <c r="D139" t="s">
         <v>294</v>
       </c>
-      <c r="C139" t="s">
-        <v>294</v>
-      </c>
-      <c r="D139" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B140" t="s">
+        <v>297</v>
+      </c>
+      <c r="C140" t="s">
+        <v>297</v>
+      </c>
+      <c r="D140" t="s">
         <v>296</v>
       </c>
-      <c r="C140" t="s">
-        <v>296</v>
-      </c>
-      <c r="D140" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B141" t="s">
+        <v>299</v>
+      </c>
+      <c r="C141" t="s">
+        <v>299</v>
+      </c>
+      <c r="D141" t="s">
         <v>298</v>
       </c>
-      <c r="C141" t="s">
-        <v>298</v>
-      </c>
-      <c r="D141" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B142" t="s">
+        <v>301</v>
+      </c>
+      <c r="C142" t="s">
+        <v>301</v>
+      </c>
+      <c r="D142" t="s">
         <v>300</v>
       </c>
-      <c r="C142" t="s">
-        <v>300</v>
-      </c>
-      <c r="D142" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B143" t="s">
+        <v>303</v>
+      </c>
+      <c r="C143" t="s">
+        <v>303</v>
+      </c>
+      <c r="D143" t="s">
         <v>302</v>
       </c>
-      <c r="C143" t="s">
-        <v>302</v>
-      </c>
-      <c r="D143" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B144" t="s">
+        <v>305</v>
+      </c>
+      <c r="C144" t="s">
+        <v>305</v>
+      </c>
+      <c r="D144" t="s">
         <v>304</v>
       </c>
-      <c r="C144" t="s">
-        <v>304</v>
-      </c>
-      <c r="D144" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B145" t="s">
+        <v>307</v>
+      </c>
+      <c r="C145" t="s">
+        <v>308</v>
+      </c>
+      <c r="D145" t="s">
         <v>306</v>
       </c>
-      <c r="C145" t="s">
-        <v>307</v>
-      </c>
-      <c r="D145" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B146" t="s">
+        <v>310</v>
+      </c>
+      <c r="C146" t="s">
+        <v>311</v>
+      </c>
+      <c r="D146" t="s">
         <v>309</v>
       </c>
-      <c r="C146" t="s">
-        <v>310</v>
-      </c>
-      <c r="D146" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B147" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C147" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D147" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B148" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="C148" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="D148" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.35">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="B149" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="C149" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D149" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.35">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B150" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="C150" t="s">
+        <v>321</v>
+      </c>
+      <c r="D150" t="s">
         <v>319</v>
       </c>
-      <c r="D150" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B151" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="C151" t="s">
+        <v>324</v>
+      </c>
+      <c r="D151" t="s">
         <v>322</v>
       </c>
-      <c r="D151" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B152" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="C152" t="s">
+        <v>327</v>
+      </c>
+      <c r="D152" t="s">
         <v>325</v>
       </c>
-      <c r="D152" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B153" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="C153" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="D153" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.35">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="B154" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="C154" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="D154" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.35">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="B155" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="C155" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="D155" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.35">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="B156" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C156" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D156" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.35">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B157" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="C157" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D157" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.35">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="B158" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C158" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="D158" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.35">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="B159" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="C159" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="D159" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.35">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="B160" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="C160" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="D160" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.35">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="B161" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="C161" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="D161" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.35">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="B162" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="C162" t="s">
+        <v>348</v>
+      </c>
+      <c r="D162" t="s">
         <v>346</v>
       </c>
-      <c r="D162" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="B163" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="C163" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="D163" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.35">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B164" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="C164" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="D164" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.35">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B165" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="C165" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="D165" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.35">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="B166" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="C166" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="D166" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.35">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B167" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="C167" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="D167" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.35">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B168" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="C168" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="D168" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.35">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="B169" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="C169" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="D169" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.35">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="B170" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C170" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="D170" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.35">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="B171" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="C171" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="D171" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.35">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="B172" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="C172" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="D172" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.35">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="B173" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="C173" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="D173" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.35">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="B174" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="C174" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="D174" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.35">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="B175" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="C175" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="D175" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.35">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="B176" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="C176" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="D176" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.35">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="B177" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="C177" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="D177" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.35">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="B178" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="C178" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="D178" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.35">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="B179" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="C179" t="s">
+        <v>383</v>
+      </c>
+      <c r="D179" t="s">
         <v>381</v>
       </c>
-      <c r="D179" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="B180" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="C180" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="D180" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.35">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="B181" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="C181" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="D181" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.35">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="B182" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="C182" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="D182" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.35">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="B183" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="C183" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="D183" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.35">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="B184" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="C184" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D184" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.35">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="B185" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="C185" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="D185" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.35">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="B186" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="C186" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="D186" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.35">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="B187" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="C187" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="D187" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.35">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="B188" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="C188" t="s">
+        <v>402</v>
+      </c>
+      <c r="D188" t="s">
         <v>400</v>
       </c>
-      <c r="D188" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="B189" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="C189" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="D189" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.35">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="B190" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="C190" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D190" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.35">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="B191" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="C191" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="D191" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.35">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="B192" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="C192" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="D192" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.35">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="B193" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C193" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="D193" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.35">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="B194" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="C194" t="s">
+        <v>415</v>
+      </c>
+      <c r="D194" t="s">
         <v>413</v>
       </c>
-      <c r="D194" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="B195" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="C195" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="D195" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.35">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="B196" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="C196" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="D196" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.35">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="B197" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="C197" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="D197" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.35">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="B198" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="C198" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="D198" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.35">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="B199" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="C199" t="s">
+        <v>426</v>
+      </c>
+      <c r="D199" t="s">
         <v>424</v>
       </c>
-      <c r="D199" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="B200" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="C200" t="s">
+        <v>429</v>
+      </c>
+      <c r="D200" t="s">
         <v>427</v>
       </c>
-      <c r="D200" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="B201" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="C201" t="s">
+        <v>432</v>
+      </c>
+      <c r="D201" t="s">
         <v>430</v>
       </c>
-      <c r="D201" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="B202" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="C202" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="D202" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.35">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="B203" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="C203" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="D203" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
     </row>
   </sheetData>

</xml_diff>